<commit_message>
add total to cash flow analysis
</commit_message>
<xml_diff>
--- a/fxms.xlsx
+++ b/fxms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazeedalkhalaf/dev/my-projects/swe-301/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C4A1F41-A70A-504B-8547-00FCC9CCDEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ACFEE0-07CF-9A48-9B8E-FC95CF013316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17220" activeTab="4" xr2:uid="{84B9E77D-7B67-B847-849D-811698F2D6F7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>project tenor</t>
   </si>
@@ -324,7 +324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +355,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -383,12 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -401,57 +401,33 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -483,10 +459,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,7 +823,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>0.15</v>
       </c>
       <c r="C5" t="s">
@@ -862,7 +834,7 @@
       <c r="A6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>0.1</v>
       </c>
       <c r="C6" t="s">
@@ -893,15 +865,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1038,7 +1010,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89D2FAA-0319-B04F-88B5-73163FF5F9AF}">
-  <dimension ref="A1:BI21"/>
+  <dimension ref="A2:BI21"/>
   <sheetViews>
     <sheetView zoomScale="65" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="Z4" activePane="bottomRight" state="frozen"/>
@@ -1063,77 +1035,63 @@
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-    </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="N2" s="11">
+      <c r="N2" s="25">
         <v>2025</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11">
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25">
         <v>2026</v>
       </c>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11">
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25">
         <v>2027</v>
       </c>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11"/>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11"/>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11"/>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="11"/>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11">
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="25"/>
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
+      <c r="AV2" s="25"/>
+      <c r="AW2" s="25"/>
+      <c r="AX2" s="25">
         <v>2028</v>
       </c>
-      <c r="AY2" s="11"/>
-      <c r="AZ2" s="11"/>
-      <c r="BA2" s="11"/>
-      <c r="BB2" s="11"/>
-      <c r="BC2" s="11"/>
-      <c r="BD2" s="11"/>
-      <c r="BE2" s="11"/>
-      <c r="BF2" s="11"/>
-      <c r="BG2" s="11"/>
-      <c r="BH2" s="11"/>
-      <c r="BI2" s="11"/>
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2" s="25"/>
+      <c r="BB2" s="25"/>
+      <c r="BC2" s="25"/>
+      <c r="BD2" s="25"/>
+      <c r="BE2" s="25"/>
+      <c r="BF2" s="25"/>
+      <c r="BG2" s="25"/>
+      <c r="BH2" s="25"/>
+      <c r="BI2" s="25"/>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -5087,10 +5045,10 @@
   <dimension ref="A1:AY58"/>
   <sheetViews>
     <sheetView zoomScale="68" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AO4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH25" sqref="AH25"/>
+      <selection pane="bottomRight" activeCell="AY13" sqref="AY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5101,66 +5059,66 @@
     <col min="30" max="39" width="11.5" bestFit="1" customWidth="1"/>
     <col min="40" max="49" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="C1" s="11">
+      <c r="C1" s="25">
         <v>2025</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25">
         <v>2026</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11">
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25">
         <v>2027</v>
       </c>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11">
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25">
         <v>2028</v>
       </c>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="11"/>
-      <c r="AQ1" s="11"/>
-      <c r="AR1" s="11"/>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11"/>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="11"/>
-      <c r="AX1" s="11"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="C2" s="3" t="s">
@@ -5307,7 +5265,7 @@
       <c r="AX2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="AY2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5522,7 +5480,7 @@
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
-      <c r="AY5" s="18">
+      <c r="AY5" s="16">
         <f>SUM(B5:AX5)</f>
         <v>-150000</v>
       </c>
@@ -5559,7 +5517,7 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
-      <c r="AY6" s="18">
+      <c r="AY6" s="16">
         <f>SUM(B6:AX6)</f>
         <v>-50000</v>
       </c>
@@ -5761,8 +5719,8 @@
         <f>-expenses!$B$3/12</f>
         <v>-25000</v>
       </c>
-      <c r="AY7" s="18">
-        <f>SUM(C7:AX7)</f>
+      <c r="AY7" s="16">
+        <f t="shared" ref="AY7:AY13" si="0">SUM(C7:AX7)</f>
         <v>-1200000</v>
       </c>
     </row>
@@ -5809,8 +5767,8 @@
         <f>-expenses!$B$4</f>
         <v>-5000</v>
       </c>
-      <c r="AY8" s="18">
-        <f>SUM(C8:AX8)</f>
+      <c r="AY8" s="16">
+        <f t="shared" si="0"/>
         <v>-20000</v>
       </c>
     </row>
@@ -6011,8 +5969,8 @@
         <f>-expenses!$B$5/12</f>
         <v>-916.66666666666663</v>
       </c>
-      <c r="AY9" s="18">
-        <f>SUM(C9:AX9)</f>
+      <c r="AY9" s="16">
+        <f t="shared" si="0"/>
         <v>-43999.999999999985</v>
       </c>
     </row>
@@ -6213,8 +6171,8 @@
         <f>-expenses!$B$6/12</f>
         <v>-41666.666666666664</v>
       </c>
-      <c r="AY10" s="18">
-        <f>SUM(C10:AX10)</f>
+      <c r="AY10" s="16">
+        <f t="shared" si="0"/>
         <v>-2000000.0000000014</v>
       </c>
     </row>
@@ -6415,8 +6373,8 @@
         <f>-expenses!$B$7/12</f>
         <v>-4166.666666666667</v>
       </c>
-      <c r="AY11" s="18">
-        <f>SUM(C11:AX11)</f>
+      <c r="AY11" s="16">
+        <f t="shared" si="0"/>
         <v>-199999.99999999991</v>
       </c>
     </row>
@@ -6617,8 +6575,8 @@
         <f>-expenses!$B$8/12</f>
         <v>-4166.666666666667</v>
       </c>
-      <c r="AY12" s="18">
-        <f>SUM(C12:AX12)</f>
+      <c r="AY12" s="16">
+        <f t="shared" si="0"/>
         <v>-199999.99999999991</v>
       </c>
     </row>
@@ -6819,8 +6777,8 @@
         <f>-staff!BI19</f>
         <v>-121947.50000000001</v>
       </c>
-      <c r="AY13" s="18">
-        <f>SUM(C13:AX13)</f>
+      <c r="AY13" s="16">
+        <f t="shared" si="0"/>
         <v>-5853480.0000000009</v>
       </c>
     </row>
@@ -6850,209 +6808,209 @@
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
-      <c r="AY14" s="18"/>
-    </row>
-    <row r="15" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="AY14" s="16"/>
+    </row>
+    <row r="15" spans="1:51" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <f>SUM(B5:B13)</f>
         <v>-200000</v>
       </c>
-      <c r="C15" s="18">
-        <f t="shared" ref="C15:AX15" si="0">SUM(C5:C13)</f>
+      <c r="C15" s="16">
+        <f t="shared" ref="C15:AX15" si="1">SUM(C5:C13)</f>
         <v>-202864.16666666669</v>
       </c>
-      <c r="D15" s="18">
-        <f t="shared" si="0"/>
+      <c r="D15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="E15" s="18">
-        <f t="shared" si="0"/>
+      <c r="E15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="F15" s="18">
-        <f t="shared" si="0"/>
+      <c r="F15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="G15" s="18">
-        <f t="shared" si="0"/>
+      <c r="G15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="H15" s="18">
-        <f t="shared" si="0"/>
+      <c r="H15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="I15" s="18">
-        <f t="shared" si="0"/>
+      <c r="I15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="J15" s="18">
-        <f t="shared" si="0"/>
+      <c r="J15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="K15" s="18">
-        <f t="shared" si="0"/>
+      <c r="K15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="L15" s="18">
-        <f t="shared" si="0"/>
+      <c r="L15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="M15" s="18">
-        <f t="shared" si="0"/>
+      <c r="M15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="N15" s="18">
-        <f t="shared" si="0"/>
+      <c r="N15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="O15" s="18">
-        <f t="shared" si="0"/>
+      <c r="O15" s="16">
+        <f t="shared" si="1"/>
         <v>-202864.16666666669</v>
       </c>
-      <c r="P15" s="18">
-        <f t="shared" si="0"/>
+      <c r="P15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="Q15" s="18">
-        <f t="shared" si="0"/>
+      <c r="Q15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="R15" s="18">
-        <f t="shared" si="0"/>
+      <c r="R15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="S15" s="18">
-        <f t="shared" si="0"/>
+      <c r="S15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="T15" s="18">
-        <f t="shared" si="0"/>
+      <c r="T15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="U15" s="18">
-        <f t="shared" si="0"/>
+      <c r="U15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="V15" s="18">
-        <f t="shared" si="0"/>
+      <c r="V15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="W15" s="18">
-        <f t="shared" si="0"/>
+      <c r="W15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="X15" s="18">
-        <f t="shared" si="0"/>
+      <c r="X15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="Y15" s="18">
-        <f t="shared" si="0"/>
+      <c r="Y15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="Z15" s="18">
-        <f t="shared" si="0"/>
+      <c r="Z15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AA15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AA15" s="16">
+        <f t="shared" si="1"/>
         <v>-202864.16666666669</v>
       </c>
-      <c r="AB15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AB15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AC15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AC15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AD15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AD15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AE15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AE15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AF15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AF15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AG15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AG15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AH15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AH15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AI15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AI15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AJ15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AJ15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AK15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AK15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AL15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AL15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AM15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AM15" s="16">
+        <f t="shared" si="1"/>
         <v>-202864.16666666669</v>
       </c>
-      <c r="AN15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AN15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AO15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AO15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AP15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AP15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AQ15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AQ15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AR15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AR15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AS15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AS15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AT15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AT15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AU15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AU15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AV15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AV15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AW15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AW15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AX15" s="18">
-        <f t="shared" si="0"/>
+      <c r="AX15" s="16">
+        <f t="shared" si="1"/>
         <v>-197864.16666666669</v>
       </c>
-      <c r="AY15" s="18">
+      <c r="AY15" s="16">
         <f>SUM(C15:AX15)</f>
         <v>-9517480.0000000019</v>
       </c>
@@ -7146,13 +7104,13 @@
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
-      <c r="AY18" s="18">
+      <c r="AY18" s="16">
         <f>SUM(B18:AX18)</f>
         <v>2000000</v>
       </c>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="9"/>
@@ -7311,7 +7269,7 @@
         <f>AW19*(1+assumption!$B$5)</f>
         <v>6658776.1711195996</v>
       </c>
-      <c r="AY19" s="18">
+      <c r="AY19" s="16">
         <f>SUM(O19:AX19)</f>
         <v>50717283.978583619</v>
       </c>
@@ -7405,212 +7363,212 @@
       <c r="AV20" s="9"/>
       <c r="AW20" s="9"/>
       <c r="AX20" s="9"/>
-      <c r="AY20" s="18">
+      <c r="AY20" s="16">
         <f>SUM(C20:AX20)</f>
         <v>3207642.5650815018</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:51" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <f>SUM(B18:B20)</f>
         <v>2000000</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="16">
         <f>SUM(C18:C20)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="18">
-        <f t="shared" ref="D22:AX22" si="1">SUM(D18:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="18">
-        <f t="shared" si="1"/>
+      <c r="D22" s="16">
+        <f t="shared" ref="D22:AX22" si="2">SUM(D18:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="16">
+        <f t="shared" si="2"/>
         <v>200000</v>
       </c>
-      <c r="P22" s="18">
-        <f t="shared" si="1"/>
+      <c r="P22" s="16">
+        <f t="shared" si="2"/>
         <v>222500</v>
       </c>
-      <c r="Q22" s="18">
-        <f t="shared" si="1"/>
+      <c r="Q22" s="16">
+        <f t="shared" si="2"/>
         <v>247625</v>
       </c>
-      <c r="R22" s="18">
-        <f t="shared" si="1"/>
+      <c r="R22" s="16">
+        <f t="shared" si="2"/>
         <v>275693.75</v>
       </c>
-      <c r="S22" s="18">
-        <f t="shared" si="1"/>
+      <c r="S22" s="16">
+        <f t="shared" si="2"/>
         <v>307065.31250000006</v>
       </c>
-      <c r="T22" s="18">
-        <f t="shared" si="1"/>
+      <c r="T22" s="16">
+        <f t="shared" si="2"/>
         <v>342144.35937500006</v>
       </c>
-      <c r="U22" s="18">
-        <f t="shared" si="1"/>
+      <c r="U22" s="16">
+        <f t="shared" si="2"/>
         <v>381387.18828125007</v>
       </c>
-      <c r="V22" s="18">
-        <f t="shared" si="1"/>
+      <c r="V22" s="16">
+        <f t="shared" si="2"/>
         <v>425308.55902343756</v>
       </c>
-      <c r="W22" s="18">
-        <f t="shared" si="1"/>
+      <c r="W22" s="16">
+        <f t="shared" si="2"/>
         <v>474489.46462695324</v>
       </c>
-      <c r="X22" s="18">
-        <f t="shared" si="1"/>
+      <c r="X22" s="16">
+        <f t="shared" si="2"/>
         <v>529585.96824599616</v>
       </c>
-      <c r="Y22" s="18">
-        <f t="shared" si="1"/>
+      <c r="Y22" s="16">
+        <f t="shared" si="2"/>
         <v>591339.25580039562</v>
       </c>
-      <c r="Z22" s="18">
-        <f t="shared" si="1"/>
+      <c r="Z22" s="16">
+        <f t="shared" si="2"/>
         <v>660587.07571970497</v>
       </c>
-      <c r="AA22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AA22" s="16">
+        <f t="shared" si="2"/>
         <v>267512.50527368532</v>
       </c>
-      <c r="AB22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AB22" s="16">
+        <f t="shared" si="2"/>
         <v>307639.38106473809</v>
       </c>
-      <c r="AC22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AC22" s="16">
+        <f t="shared" si="2"/>
         <v>353785.2882244488</v>
       </c>
-      <c r="AD22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AD22" s="16">
+        <f t="shared" si="2"/>
         <v>406853.08145811607</v>
       </c>
-      <c r="AE22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AE22" s="16">
+        <f t="shared" si="2"/>
         <v>467881.04367683345</v>
       </c>
-      <c r="AF22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AF22" s="16">
+        <f t="shared" si="2"/>
         <v>538063.20022835839</v>
       </c>
-      <c r="AG22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AG22" s="16">
+        <f t="shared" si="2"/>
         <v>618772.68026261206</v>
       </c>
-      <c r="AH22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AH22" s="16">
+        <f t="shared" si="2"/>
         <v>711588.58230200387</v>
       </c>
-      <c r="AI22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AI22" s="16">
+        <f t="shared" si="2"/>
         <v>818326.86964730441</v>
       </c>
-      <c r="AJ22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AJ22" s="16">
+        <f t="shared" si="2"/>
         <v>941075.90009440004</v>
       </c>
-      <c r="AK22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AK22" s="16">
+        <f t="shared" si="2"/>
         <v>1082237.28510856</v>
       </c>
-      <c r="AL22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AL22" s="16">
+        <f t="shared" si="2"/>
         <v>1244572.877874844</v>
       </c>
-      <c r="AM22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AM22" s="16">
+        <f t="shared" si="2"/>
         <v>1431258.8095560705</v>
       </c>
-      <c r="AN22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AN22" s="16">
+        <f t="shared" si="2"/>
         <v>1645947.630989481</v>
       </c>
-      <c r="AO22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AO22" s="16">
+        <f t="shared" si="2"/>
         <v>1892839.775637903</v>
       </c>
-      <c r="AP22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AP22" s="16">
+        <f t="shared" si="2"/>
         <v>2176765.7419835883</v>
       </c>
-      <c r="AQ22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AQ22" s="16">
+        <f t="shared" si="2"/>
         <v>2503280.6032811264</v>
       </c>
-      <c r="AR22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AR22" s="16">
+        <f t="shared" si="2"/>
         <v>2878772.6937732953</v>
       </c>
-      <c r="AS22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AS22" s="16">
+        <f t="shared" si="2"/>
         <v>3310588.5978392893</v>
       </c>
-      <c r="AT22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AT22" s="16">
+        <f t="shared" si="2"/>
         <v>3807176.8875151826</v>
       </c>
-      <c r="AU22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AU22" s="16">
+        <f t="shared" si="2"/>
         <v>4378253.4206424598</v>
       </c>
-      <c r="AV22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AV22" s="16">
+        <f t="shared" si="2"/>
         <v>5034991.4337388286</v>
       </c>
-      <c r="AW22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AW22" s="16">
+        <f t="shared" si="2"/>
         <v>5790240.1487996522</v>
       </c>
-      <c r="AX22" s="18">
-        <f t="shared" si="1"/>
+      <c r="AX22" s="16">
+        <f t="shared" si="2"/>
         <v>6658776.1711195996</v>
       </c>
-      <c r="AY22" s="18">
+      <c r="AY22" s="16">
         <f>SUM(B22:AX22)</f>
         <v>55924926.543665111</v>
       </c>
@@ -7651,198 +7609,198 @@
         <v>1800000</v>
       </c>
       <c r="C24" s="9">
-        <f t="shared" ref="C24:AX24" si="2">C15+C22</f>
+        <f t="shared" ref="C24:AX24" si="3">C15+C22</f>
         <v>-202864.16666666669</v>
       </c>
       <c r="D24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="F24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="L24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="N24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-197864.16666666669</v>
       </c>
       <c r="O24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2864.1666666666861</v>
       </c>
       <c r="P24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24635.833333333314</v>
       </c>
       <c r="Q24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49760.833333333314</v>
       </c>
       <c r="R24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77829.583333333314</v>
       </c>
       <c r="S24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109201.14583333337</v>
       </c>
       <c r="T24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>144280.19270833337</v>
       </c>
       <c r="U24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>183523.02161458338</v>
       </c>
       <c r="V24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>227444.39235677087</v>
       </c>
       <c r="W24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>276625.29796028655</v>
       </c>
       <c r="X24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>331721.80157932948</v>
       </c>
       <c r="Y24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>393475.08913372894</v>
       </c>
       <c r="Z24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>462722.90905303828</v>
       </c>
       <c r="AA24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64648.338607018639</v>
       </c>
       <c r="AB24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>109775.2143980714</v>
       </c>
       <c r="AC24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>155921.12155778211</v>
       </c>
       <c r="AD24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208988.91479144938</v>
       </c>
       <c r="AE24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>270016.87701016676</v>
       </c>
       <c r="AF24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>340199.0335616917</v>
       </c>
       <c r="AG24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>420908.51359594538</v>
       </c>
       <c r="AH24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>513724.41563533718</v>
       </c>
       <c r="AI24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>620462.70298063778</v>
       </c>
       <c r="AJ24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>743211.73342773342</v>
       </c>
       <c r="AK24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>884373.11844189325</v>
       </c>
       <c r="AL24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1046708.7112081773</v>
       </c>
       <c r="AM24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1228394.6428894037</v>
       </c>
       <c r="AN24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1448083.4643228143</v>
       </c>
       <c r="AO24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1694975.6089712363</v>
       </c>
       <c r="AP24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1978901.5753169216</v>
       </c>
       <c r="AQ24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2305416.4366144598</v>
       </c>
       <c r="AR24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2680908.5271066288</v>
       </c>
       <c r="AS24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3112724.4311726228</v>
       </c>
       <c r="AT24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3609312.7208485161</v>
       </c>
       <c r="AU24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4180389.2539757933</v>
       </c>
       <c r="AV24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4837127.2670721617</v>
       </c>
       <c r="AW24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5592375.9821329853</v>
       </c>
       <c r="AX24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6460912.0044529326</v>
       </c>
-      <c r="AY24" s="18"/>
+      <c r="AY24" s="16"/>
     </row>
     <row r="25" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
@@ -7857,187 +7815,187 @@
         <v>1597135.8333333333</v>
       </c>
       <c r="D25" s="9">
-        <f t="shared" ref="D25:Z25" si="3">D24+C25</f>
+        <f t="shared" ref="D25:Z25" si="4">D24+C25</f>
         <v>1399271.6666666665</v>
       </c>
       <c r="E25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1201407.4999999998</v>
       </c>
       <c r="F25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1003543.333333333</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>805679.16666666628</v>
       </c>
       <c r="H25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>607814.99999999953</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>409950.83333333285</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>212086.66666666616</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14222.499999999476</v>
       </c>
       <c r="L25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-183641.66666666721</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-381505.8333333339</v>
       </c>
       <c r="N25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-579370.00000000058</v>
       </c>
       <c r="O25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-582234.16666666721</v>
       </c>
       <c r="P25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-557598.33333333395</v>
       </c>
       <c r="Q25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-507837.50000000064</v>
       </c>
       <c r="R25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-430007.91666666733</v>
       </c>
       <c r="S25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-320806.77083333395</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-176526.57812500058</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6996.4434895828017</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234440.83584635367</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>511066.13380664022</v>
       </c>
       <c r="X25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>842787.9353859697</v>
       </c>
       <c r="Y25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1236263.0245196987</v>
       </c>
       <c r="Z25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1698985.933572737</v>
       </c>
       <c r="AA25" s="9">
-        <f t="shared" ref="AA25" si="4">AA24+Z25</f>
+        <f t="shared" ref="AA25" si="5">AA24+Z25</f>
         <v>1763634.2721797556</v>
       </c>
       <c r="AB25" s="9">
-        <f t="shared" ref="AB25" si="5">AB24+AA25</f>
+        <f t="shared" ref="AB25" si="6">AB24+AA25</f>
         <v>1873409.486577827</v>
       </c>
       <c r="AC25" s="9">
-        <f t="shared" ref="AC25" si="6">AC24+AB25</f>
+        <f t="shared" ref="AC25" si="7">AC24+AB25</f>
         <v>2029330.6081356092</v>
       </c>
       <c r="AD25" s="9">
-        <f t="shared" ref="AD25" si="7">AD24+AC25</f>
+        <f t="shared" ref="AD25" si="8">AD24+AC25</f>
         <v>2238319.5229270584</v>
       </c>
       <c r="AE25" s="9">
-        <f t="shared" ref="AE25" si="8">AE24+AD25</f>
+        <f t="shared" ref="AE25" si="9">AE24+AD25</f>
         <v>2508336.399937225</v>
       </c>
       <c r="AF25" s="9">
-        <f t="shared" ref="AF25" si="9">AF24+AE25</f>
+        <f t="shared" ref="AF25" si="10">AF24+AE25</f>
         <v>2848535.4334989167</v>
       </c>
       <c r="AG25" s="9">
-        <f t="shared" ref="AG25" si="10">AG24+AF25</f>
+        <f t="shared" ref="AG25" si="11">AG24+AF25</f>
         <v>3269443.9470948619</v>
       </c>
       <c r="AH25" s="9">
-        <f t="shared" ref="AH25" si="11">AH24+AG25</f>
+        <f t="shared" ref="AH25" si="12">AH24+AG25</f>
         <v>3783168.362730199</v>
       </c>
       <c r="AI25" s="9">
-        <f t="shared" ref="AI25" si="12">AI24+AH25</f>
+        <f t="shared" ref="AI25" si="13">AI24+AH25</f>
         <v>4403631.065710837</v>
       </c>
       <c r="AJ25" s="9">
-        <f t="shared" ref="AJ25" si="13">AJ24+AI25</f>
+        <f t="shared" ref="AJ25" si="14">AJ24+AI25</f>
         <v>5146842.7991385702</v>
       </c>
       <c r="AK25" s="9">
-        <f t="shared" ref="AK25" si="14">AK24+AJ25</f>
+        <f t="shared" ref="AK25" si="15">AK24+AJ25</f>
         <v>6031215.917580463</v>
       </c>
       <c r="AL25" s="9">
-        <f t="shared" ref="AL25" si="15">AL24+AK25</f>
+        <f t="shared" ref="AL25" si="16">AL24+AK25</f>
         <v>7077924.6287886407</v>
       </c>
       <c r="AM25" s="9">
-        <f t="shared" ref="AM25" si="16">AM24+AL25</f>
+        <f t="shared" ref="AM25" si="17">AM24+AL25</f>
         <v>8306319.2716780445</v>
       </c>
       <c r="AN25" s="9">
-        <f t="shared" ref="AN25" si="17">AN24+AM25</f>
+        <f t="shared" ref="AN25" si="18">AN24+AM25</f>
         <v>9754402.7360008582</v>
       </c>
       <c r="AO25" s="9">
-        <f t="shared" ref="AO25" si="18">AO24+AN25</f>
+        <f t="shared" ref="AO25" si="19">AO24+AN25</f>
         <v>11449378.344972095</v>
       </c>
       <c r="AP25" s="9">
-        <f t="shared" ref="AP25" si="19">AP24+AO25</f>
+        <f t="shared" ref="AP25" si="20">AP24+AO25</f>
         <v>13428279.920289015</v>
       </c>
       <c r="AQ25" s="9">
-        <f t="shared" ref="AQ25" si="20">AQ24+AP25</f>
+        <f t="shared" ref="AQ25" si="21">AQ24+AP25</f>
         <v>15733696.356903475</v>
       </c>
       <c r="AR25" s="9">
-        <f t="shared" ref="AR25" si="21">AR24+AQ25</f>
+        <f t="shared" ref="AR25" si="22">AR24+AQ25</f>
         <v>18414604.884010103</v>
       </c>
       <c r="AS25" s="9">
-        <f t="shared" ref="AS25" si="22">AS24+AR25</f>
+        <f t="shared" ref="AS25" si="23">AS24+AR25</f>
         <v>21527329.315182727</v>
       </c>
       <c r="AT25" s="9">
-        <f t="shared" ref="AT25" si="23">AT24+AS25</f>
+        <f t="shared" ref="AT25" si="24">AT24+AS25</f>
         <v>25136642.036031242</v>
       </c>
       <c r="AU25" s="9">
-        <f t="shared" ref="AU25" si="24">AU24+AT25</f>
+        <f t="shared" ref="AU25" si="25">AU24+AT25</f>
         <v>29317031.290007036</v>
       </c>
       <c r="AV25" s="9">
-        <f t="shared" ref="AV25" si="25">AV24+AU25</f>
+        <f t="shared" ref="AV25" si="26">AV24+AU25</f>
         <v>34154158.557079196</v>
       </c>
       <c r="AW25" s="9">
-        <f t="shared" ref="AW25" si="26">AW24+AV25</f>
+        <f t="shared" ref="AW25" si="27">AW24+AV25</f>
         <v>39746534.539212182</v>
       </c>
     </row>
@@ -8121,10 +8079,10 @@
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
-      <c r="AW28" s="21" t="s">
+      <c r="AW28" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AX28" s="15">
+      <c r="AX28" s="13">
         <f>SUM(AY22,AY15)/-AY15</f>
         <v>4.8760224916327752</v>
       </c>
@@ -8153,7 +8111,7 @@
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
-      <c r="AW29" s="21" t="s">
+      <c r="AW29" s="18" t="s">
         <v>57</v>
       </c>
       <c r="AX29" s="9">
@@ -8949,7 +8907,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B25:AW25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8966,7 +8924,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8975,78 +8933,37 @@
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="29" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="27" t="s">
+        <v>9</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -9090,7 +9007,7 @@
       <c r="AV2" s="3"/>
       <c r="AW2" s="3"/>
       <c r="AX2" s="3"/>
-      <c r="AY2" s="27"/>
+      <c r="AY2" s="12"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
@@ -9109,10 +9026,9 @@
       <c r="F3" s="5">
         <v>4</v>
       </c>
-      <c r="AY3" s="26"/>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="20" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4"/>
@@ -9120,7 +9036,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -9169,7 +9085,7 @@
       <c r="BA4" s="4"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4">
@@ -9180,7 +9096,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="29">
+        <f>SUM(B5:F5)</f>
+        <v>-150000</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -9229,7 +9148,7 @@
       <c r="BA5" s="4"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="4">
@@ -9240,7 +9159,10 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="29">
+        <f t="shared" ref="G6:G13" si="0">SUM(B6:F6)</f>
+        <v>-50000</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -9289,7 +9211,7 @@
       <c r="BA6" s="4"/>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4"/>
@@ -9309,7 +9231,10 @@
         <f>SUM(cashflow!AM7:AX7)</f>
         <v>-300000</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="29">
+        <f t="shared" si="0"/>
+        <v>-1200000</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -9358,7 +9283,7 @@
       <c r="BA7" s="4"/>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="4"/>
@@ -9378,7 +9303,10 @@
         <f>SUM(cashflow!AM8:AX8)</f>
         <v>-5000</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="29">
+        <f t="shared" si="0"/>
+        <v>-20000</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -9427,7 +9355,7 @@
       <c r="BA8" s="4"/>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="4"/>
@@ -9447,7 +9375,10 @@
         <f>SUM(cashflow!AM9:AX9)</f>
         <v>-10999.999999999998</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="29">
+        <f t="shared" si="0"/>
+        <v>-43999.999999999993</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -9496,7 +9427,7 @@
       <c r="BA9" s="4"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="4"/>
@@ -9516,7 +9447,10 @@
         <f>SUM(cashflow!AM10:AX10)</f>
         <v>-500000.00000000006</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="29">
+        <f t="shared" si="0"/>
+        <v>-2000000.0000000002</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -9565,7 +9499,7 @@
       <c r="BA10" s="4"/>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="4"/>
@@ -9585,7 +9519,10 @@
         <f>SUM(cashflow!AM11:AX11)</f>
         <v>-49999.999999999993</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="29">
+        <f t="shared" si="0"/>
+        <v>-199999.99999999997</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -9634,7 +9571,7 @@
       <c r="BA11" s="4"/>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="4"/>
@@ -9654,7 +9591,10 @@
         <f>SUM(cashflow!AM12:AX12)</f>
         <v>-49999.999999999993</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="29">
+        <f t="shared" si="0"/>
+        <v>-199999.99999999997</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -9703,7 +9643,7 @@
       <c r="BA12" s="4"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="4"/>
@@ -9723,7 +9663,10 @@
         <f>SUM(cashflow!AM13:AX13)</f>
         <v>-1463370.0000000002</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="29">
+        <f t="shared" si="0"/>
+        <v>-5853480.0000000009</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -9772,13 +9715,13 @@
       <c r="BA13" s="4"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -9827,30 +9770,33 @@
       <c r="BA14" s="4"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="23">
         <f>SUM(B5:B13)</f>
         <v>-200000</v>
       </c>
-      <c r="C15" s="28">
-        <f t="shared" ref="C15:F15" si="0">SUM(C5:C13)</f>
+      <c r="C15" s="23">
+        <f t="shared" ref="C15:F15" si="1">SUM(C5:C13)</f>
         <v>-2379370</v>
       </c>
-      <c r="D15" s="28">
-        <f t="shared" si="0"/>
+      <c r="D15" s="23">
+        <f t="shared" si="1"/>
         <v>-2379370</v>
       </c>
-      <c r="E15" s="28">
-        <f t="shared" si="0"/>
+      <c r="E15" s="23">
+        <f t="shared" si="1"/>
         <v>-2379370</v>
       </c>
-      <c r="F15" s="28">
-        <f t="shared" si="0"/>
+      <c r="F15" s="23">
+        <f t="shared" si="1"/>
         <v>-2379370</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="29">
+        <f>SUM(B15:F15)</f>
+        <v>-9717480</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -9899,13 +9845,13 @@
       <c r="BA15" s="4"/>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -9954,7 +9900,7 @@
       <c r="BA16" s="4"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
@@ -9962,7 +9908,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -10011,7 +9957,7 @@
       <c r="BA17" s="4"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="4">
@@ -10022,7 +9968,10 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="29">
+        <f>SUM(B18:F18)</f>
+        <v>2000000</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -10071,7 +10020,7 @@
       <c r="BA18" s="4"/>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="4"/>
@@ -10088,7 +10037,10 @@
         <f>SUM(cashflow!AM19:AX19)</f>
         <v>41508891.914876476</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="29">
+        <f t="shared" ref="G19:G20" si="2">SUM(B19:F19)</f>
+        <v>50717283.978583619</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -10137,7 +10089,7 @@
       <c r="BA19" s="4"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B20" s="4"/>
@@ -10154,7 +10106,10 @@
         <f>SUM(cashflow!AM20:AX20)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="29">
+        <f t="shared" si="2"/>
+        <v>3207642.5650815018</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -10203,13 +10158,13 @@
       <c r="BA20" s="4"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -10258,30 +10213,33 @@
       <c r="BA21" s="4"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="23">
         <f>SUM(B18:B20)</f>
         <v>2000000</v>
       </c>
-      <c r="C22" s="28">
-        <f t="shared" ref="C22:F22" si="1">SUM(C18:C20)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="28">
-        <f t="shared" si="1"/>
+      <c r="C22" s="23">
+        <f t="shared" ref="C22:F22" si="3">SUM(C18:C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="23">
+        <f t="shared" si="3"/>
         <v>4657725.9335727375</v>
       </c>
-      <c r="E22" s="28">
-        <f t="shared" si="1"/>
+      <c r="E22" s="23">
+        <f t="shared" si="3"/>
         <v>7758308.6952159042</v>
       </c>
-      <c r="F22" s="28">
-        <f t="shared" si="1"/>
+      <c r="F22" s="23">
+        <f t="shared" si="3"/>
         <v>41508891.914876476</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="29">
+        <f>SUM(B22:F22)</f>
+        <v>55924926.543665119</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -10330,13 +10288,13 @@
       <c r="BA22" s="4"/>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -10385,7 +10343,7 @@
       <c r="BA23" s="4"/>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="4">
@@ -10393,22 +10351,25 @@
         <v>1800000</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" ref="C24:F24" si="2">C15+C22</f>
+        <f t="shared" ref="C24:F24" si="4">C15+C22</f>
         <v>-2379370</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2278355.9335727375</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5378938.6952159042</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39129521.914876476</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="29">
+        <f>SUM(B24:F24)</f>
+        <v>46207446.543665119</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -10457,7 +10418,7 @@
       <c r="BA24" s="4"/>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="4">
@@ -10469,18 +10430,18 @@
         <v>-579370</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" ref="D25:F25" si="3">D24+C25</f>
+        <f t="shared" ref="D25:F25" si="5">D24+C25</f>
         <v>1698985.9335727375</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7077924.6287886417</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>46207446.543665119</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -10534,7 +10495,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="29"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -10588,7 +10549,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -10642,7 +10603,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -10696,7 +10657,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -10750,7 +10711,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -10804,7 +10765,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -10858,7 +10819,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -10912,7 +10873,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="29"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -10966,7 +10927,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="29"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -11020,7 +10981,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="29"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -11074,7 +11035,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="29"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -11128,7 +11089,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -11182,7 +11143,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -11236,7 +11197,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -11290,7 +11251,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="29"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -11344,7 +11305,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="29"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -11398,7 +11359,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="29"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -11452,7 +11413,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -11506,7 +11467,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -11560,7 +11521,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="29"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -11614,7 +11575,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="G46" s="29"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -11668,7 +11629,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="G47" s="29"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
@@ -11722,7 +11683,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="G48" s="29"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -11802,16 +11763,11 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A25:XFD25">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>